<commit_message>
Added test error estimation using cross-validation
</commit_message>
<xml_diff>
--- a/MSE_motivation.xlsx
+++ b/MSE_motivation.xlsx
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tiss-2025\learning-isl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344409B4-CBA2-49AA-8237-07D3D885EE38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC821F29-3802-48A2-B7D7-7A250CE80893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{8519553A-6E39-4723-8F51-C21798431B9A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{8519553A-6E39-4723-8F51-C21798431B9A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="MSE" sheetId="2" r:id="rId2"/>
+    <sheet name="MSE_1" sheetId="1" r:id="rId1"/>
+    <sheet name="MSE_2" sheetId="2" r:id="rId2"/>
     <sheet name="Accuracy" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -501,193 +512,196 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8793CE4E-9C43-40C8-996B-3E986CD2749E}">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="6" max="13" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" t="s">
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>6</v>
       </c>
-      <c r="M1" t="s">
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="G2">
+        <v>230.1</v>
+      </c>
+      <c r="H2">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="I2">
+        <v>69.2</v>
+      </c>
+      <c r="J2">
+        <v>22.1</v>
+      </c>
+      <c r="K2">
+        <v>20.523974410000001</v>
+      </c>
+      <c r="L2">
+        <v>20.555464629999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
         <v>7</v>
       </c>
-      <c r="N1" t="s">
+      <c r="G3">
+        <v>44.5</v>
+      </c>
+      <c r="H3">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="I3">
+        <v>45.1</v>
+      </c>
+      <c r="J3">
+        <v>10.4</v>
+      </c>
+      <c r="K3">
+        <v>12.33785482</v>
+      </c>
+      <c r="L3">
+        <v>12.345362290000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>17.2</v>
+      </c>
+      <c r="H4">
+        <v>45.9</v>
+      </c>
+      <c r="I4">
+        <v>69.3</v>
+      </c>
+      <c r="J4">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="K4">
+        <v>12.30767078</v>
+      </c>
+      <c r="L4">
+        <v>12.337017729999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>151.5</v>
+      </c>
+      <c r="H5">
+        <v>41.3</v>
+      </c>
+      <c r="I5">
+        <v>58.5</v>
+      </c>
+      <c r="J5">
+        <v>18.5</v>
+      </c>
+      <c r="K5">
+        <v>17.59782951</v>
+      </c>
+      <c r="L5">
+        <v>17.61711596</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2">
-        <v>230.1</v>
-      </c>
-      <c r="B2">
-        <v>37.799999999999997</v>
-      </c>
-      <c r="C2">
-        <v>69.2</v>
-      </c>
-      <c r="D2">
-        <v>22.1</v>
-      </c>
-      <c r="E2">
-        <v>20.523974410000001</v>
-      </c>
-      <c r="F2">
-        <v>20.555464629999999</v>
-      </c>
-      <c r="L2">
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
         <v>4</v>
       </c>
-      <c r="M2">
-        <v>6</v>
-      </c>
-      <c r="N2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3">
-        <v>44.5</v>
-      </c>
-      <c r="B3">
-        <v>39.299999999999997</v>
-      </c>
-      <c r="C3">
-        <v>45.1</v>
-      </c>
-      <c r="D3">
-        <v>10.4</v>
-      </c>
-      <c r="E3">
-        <v>12.33785482</v>
-      </c>
-      <c r="F3">
-        <v>12.345362290000001</v>
-      </c>
-      <c r="L3">
-        <v>5</v>
-      </c>
-      <c r="M3">
-        <v>6</v>
-      </c>
-      <c r="N3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4">
-        <v>17.2</v>
-      </c>
-      <c r="B4">
-        <v>45.9</v>
-      </c>
-      <c r="C4">
-        <v>69.3</v>
-      </c>
-      <c r="D4">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="E4">
-        <v>12.30767078</v>
-      </c>
-      <c r="F4">
-        <v>12.337017729999999</v>
-      </c>
-      <c r="L4">
-        <v>6</v>
-      </c>
-      <c r="M4">
-        <v>6</v>
-      </c>
-      <c r="N4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5">
-        <v>151.5</v>
-      </c>
-      <c r="B5">
-        <v>41.3</v>
-      </c>
-      <c r="C5">
-        <v>58.5</v>
-      </c>
-      <c r="D5">
-        <v>18.5</v>
-      </c>
-      <c r="E5">
-        <v>17.59782951</v>
-      </c>
-      <c r="F5">
-        <v>17.61711596</v>
-      </c>
-      <c r="L5">
-        <v>7</v>
-      </c>
-      <c r="M5">
-        <v>6</v>
-      </c>
-      <c r="N5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6">
+      <c r="G6">
         <v>180.8</v>
       </c>
-      <c r="B6">
+      <c r="H6">
         <v>10.8</v>
       </c>
-      <c r="C6">
+      <c r="I6">
         <v>58.4</v>
       </c>
-      <c r="D6">
+      <c r="J6">
         <v>12.9</v>
       </c>
-      <c r="E6">
+      <c r="K6">
         <v>13.188671859999999</v>
       </c>
-      <c r="F6">
+      <c r="L6">
         <v>13.22390813</v>
       </c>
-      <c r="L6">
-        <v>8</v>
-      </c>
-      <c r="M6">
-        <v>6</v>
-      </c>
-      <c r="N6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="5:6">
-      <c r="E22" s="1">
+    </row>
+    <row r="22" spans="11:12">
+      <c r="K22" s="1">
         <v>3.2364000000000002</v>
       </c>
-      <c r="F22" s="1">
+      <c r="L22" s="1">
         <v>3.2555000000000001</v>
       </c>
     </row>
@@ -701,7 +715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B37EF267-053A-4427-9649-80210655C072}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>

</xml_diff>